<commit_message>
Updated cleaned data files and added rough.py
</commit_message>
<xml_diff>
--- a/last season cleaned data/allroundersetlastseason_ipl.xlsx
+++ b/last season cleaned data/allroundersetlastseason_ipl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/Dataset_Final/cleaned last season/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/cricket-squad-selection/last season cleaned data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDA36BA-A73A-F84C-9044-073121011F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32FA8B3-2F50-094F-9E12-A8D1AD5D20D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="6920" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Merged" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>Player</t>
   </si>
@@ -64,9 +64,6 @@
     <t>R Shepherd</t>
   </si>
   <si>
-    <t>39*</t>
-  </si>
-  <si>
     <t>AR</t>
   </si>
   <si>
@@ -82,15 +79,9 @@
     <t>Washington Sundar</t>
   </si>
   <si>
-    <t>0*</t>
-  </si>
-  <si>
     <t>Arshad Khan</t>
   </si>
   <si>
-    <t>58*</t>
-  </si>
-  <si>
     <t>Mohammad Nabi</t>
   </si>
   <si>
@@ -115,18 +106,12 @@
     <t>K Nitish Kumar Reddy</t>
   </si>
   <si>
-    <t>76*</t>
-  </si>
-  <si>
     <t>HH Pandya</t>
   </si>
   <si>
     <t>WG Jacks</t>
   </si>
   <si>
-    <t>100*</t>
-  </si>
-  <si>
     <t>GJ Maxwell</t>
   </si>
   <si>
@@ -136,88 +121,52 @@
     <t>Shahbaz Ahmed</t>
   </si>
   <si>
-    <t>59*</t>
-  </si>
-  <si>
     <t>MM Ali</t>
   </si>
   <si>
     <t>KH Pandya</t>
   </si>
   <si>
-    <t>43*</t>
-  </si>
-  <si>
     <t>PJ Cummins</t>
   </si>
   <si>
-    <t>35*</t>
-  </si>
-  <si>
     <t>R Sai Kishore</t>
   </si>
   <si>
     <t>LS Livingstone</t>
   </si>
   <si>
-    <t>38*</t>
-  </si>
-  <si>
     <t>Harpreet Brar</t>
   </si>
   <si>
     <t>Swapnil Singh</t>
   </si>
   <si>
-    <t>15*</t>
-  </si>
-  <si>
     <t>DG Nalkande</t>
   </si>
   <si>
     <t>RA Jadeja</t>
   </si>
   <si>
-    <t>57*</t>
-  </si>
-  <si>
     <t>AR Patel</t>
   </si>
   <si>
     <t>MP Stoinis</t>
   </si>
   <si>
-    <t>124*</t>
-  </si>
-  <si>
     <t>SM Curran</t>
   </si>
   <si>
-    <t>63*</t>
-  </si>
-  <si>
     <t>Abhishek Sharma</t>
   </si>
   <si>
-    <t>75*</t>
-  </si>
-  <si>
     <t>AD Russell</t>
   </si>
   <si>
-    <t>64*</t>
-  </si>
-  <si>
     <t>S Dube</t>
   </si>
   <si>
-    <t>66*</t>
-  </si>
-  <si>
     <t>Shashank Singh</t>
-  </si>
-  <si>
-    <t>68*</t>
   </si>
   <si>
     <t>C Green</t>
@@ -628,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -666,34 +615,34 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>6</v>
@@ -708,25 +657,25 @@
         <v>10</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>2</v>
@@ -751,8 +700,8 @@
       <c r="F2" s="1">
         <v>57</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
+      <c r="G2" s="1">
+        <v>39</v>
       </c>
       <c r="H2" s="1">
         <v>28.5</v>
@@ -806,12 +755,12 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -883,12 +832,12 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>6</v>
@@ -960,12 +909,12 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1037,12 +986,12 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -1059,8 +1008,8 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>20</v>
+      <c r="G6" s="1">
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -1114,12 +1063,12 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1136,8 +1085,8 @@
       <c r="F7" s="1">
         <v>83</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
+      <c r="G7" s="1">
+        <v>58</v>
       </c>
       <c r="H7" s="1">
         <v>41.5</v>
@@ -1191,12 +1140,12 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -1268,12 +1217,12 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1345,12 +1294,12 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -1422,12 +1371,12 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
@@ -1499,12 +1448,12 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
@@ -1576,12 +1525,12 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -1653,12 +1602,12 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -1730,12 +1679,12 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -1752,8 +1701,8 @@
       <c r="F15" s="1">
         <v>303</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>31</v>
+      <c r="G15" s="1">
+        <v>76</v>
       </c>
       <c r="H15" s="1">
         <v>33.659999999999997</v>
@@ -1807,12 +1756,12 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -1884,12 +1833,12 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
@@ -1906,8 +1855,8 @@
       <c r="F17" s="1">
         <v>230</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>34</v>
+      <c r="G17" s="1">
+        <v>100</v>
       </c>
       <c r="H17" s="1">
         <v>32.85</v>
@@ -1961,12 +1910,12 @@
         <v>0</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
@@ -2038,12 +1987,12 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>5</v>
@@ -2115,12 +2064,12 @@
         <v>0</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1">
         <v>3</v>
@@ -2137,8 +2086,8 @@
       <c r="F20" s="1">
         <v>215</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>38</v>
+      <c r="G20" s="1">
+        <v>59</v>
       </c>
       <c r="H20" s="1">
         <v>23.88</v>
@@ -2192,12 +2141,12 @@
         <v>0</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
@@ -2269,12 +2218,12 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -2291,8 +2240,8 @@
       <c r="F22" s="1">
         <v>133</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>41</v>
+      <c r="G22" s="1">
+        <v>43</v>
       </c>
       <c r="H22" s="1">
         <v>33.25</v>
@@ -2346,12 +2295,12 @@
         <v>0</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1">
         <v>7</v>
@@ -2368,8 +2317,8 @@
       <c r="F23" s="1">
         <v>136</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>43</v>
+      <c r="G23" s="1">
+        <v>35</v>
       </c>
       <c r="H23" s="1">
         <v>22.66</v>
@@ -2423,12 +2372,12 @@
         <v>0</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
@@ -2500,12 +2449,12 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
@@ -2522,8 +2471,8 @@
       <c r="F25" s="1">
         <v>111</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>46</v>
+      <c r="G25" s="1">
+        <v>38</v>
       </c>
       <c r="H25" s="1">
         <v>22.2</v>
@@ -2577,12 +2526,12 @@
         <v>0</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1">
         <v>7</v>
@@ -2654,12 +2603,12 @@
         <v>0</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1">
         <v>2</v>
@@ -2676,8 +2625,8 @@
       <c r="F27" s="1">
         <v>37</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>49</v>
+      <c r="G27" s="1">
+        <v>15</v>
       </c>
       <c r="H27" s="1">
         <v>18.5</v>
@@ -2731,12 +2680,12 @@
         <v>0</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1">
         <v>2</v>
@@ -2808,12 +2757,12 @@
         <v>0</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1">
         <v>6</v>
@@ -2830,8 +2779,8 @@
       <c r="F29" s="1">
         <v>267</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>52</v>
+      <c r="G29" s="1">
+        <v>57</v>
       </c>
       <c r="H29" s="1">
         <v>44.5</v>
@@ -2885,12 +2834,12 @@
         <v>0</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1">
         <v>13</v>
@@ -2962,12 +2911,12 @@
         <v>0</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1">
         <v>4</v>
@@ -2984,8 +2933,8 @@
       <c r="F31" s="1">
         <v>388</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>55</v>
+      <c r="G31" s="1">
+        <v>124</v>
       </c>
       <c r="H31" s="1">
         <v>32.33</v>
@@ -3039,12 +2988,12 @@
         <v>0</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B32" s="1">
         <v>7</v>
@@ -3061,8 +3010,8 @@
       <c r="F32" s="1">
         <v>270</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>57</v>
+      <c r="G32" s="1">
+        <v>63</v>
       </c>
       <c r="H32" s="1">
         <v>27</v>
@@ -3116,12 +3065,12 @@
         <v>0</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B33" s="1">
         <v>7</v>
@@ -3138,8 +3087,8 @@
       <c r="F33" s="1">
         <v>484</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>59</v>
+      <c r="G33" s="1">
+        <v>75</v>
       </c>
       <c r="H33" s="1">
         <v>32.26</v>
@@ -3193,12 +3142,12 @@
         <v>0</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1">
         <v>3</v>
@@ -3215,8 +3164,8 @@
       <c r="F34" s="1">
         <v>222</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>61</v>
+      <c r="G34" s="1">
+        <v>64</v>
       </c>
       <c r="H34" s="1">
         <v>31.71</v>
@@ -3270,12 +3219,12 @@
         <v>0</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1">
         <v>2</v>
@@ -3292,8 +3241,8 @@
       <c r="F35" s="1">
         <v>396</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>63</v>
+      <c r="G35" s="1">
+        <v>66</v>
       </c>
       <c r="H35" s="1">
         <v>36</v>
@@ -3347,12 +3296,12 @@
         <v>0</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B36" s="1">
         <v>7</v>
@@ -3369,8 +3318,8 @@
       <c r="F36" s="1">
         <v>354</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>65</v>
+      <c r="G36" s="1">
+        <v>68</v>
       </c>
       <c r="H36" s="1">
         <v>44.25</v>
@@ -3424,12 +3373,12 @@
         <v>0</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1">
         <v>5</v>

</xml_diff>